<commit_message>
Update scripts and data; ignore IDE files
</commit_message>
<xml_diff>
--- a/myotube-quant/data/Passage.xlsx
+++ b/myotube-quant/data/Passage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45a615307d5b8c65/Desktop/Lab/myotube-quant/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19CF26EE-6E78-42EC-BFC9-BC1C06773879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{19CF26EE-6E78-42EC-BFC9-BC1C06773879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E91C4DFF-D387-4BE2-B258-18C056CBC084}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8AD0EC4-18FE-402D-AD88-18FAD9E7B5FE}"/>
+    <workbookView xWindow="0" yWindow="576" windowWidth="11856" windowHeight="10428" xr2:uid="{E8AD0EC4-18FE-402D-AD88-18FAD9E7B5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,21 +457,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA977DA-E8AC-4FF6-9979-EF81329F4272}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
     <col min="2" max="2" width="6.109375" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="42.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>